<commit_message>
update excel url with blob
</commit_message>
<xml_diff>
--- a/techniques-copia.xlsx
+++ b/techniques-copia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\Documents\UPC - Ingeniería de Software\Ciclo 9\TP1\RelaxationTechniques\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\Documents\UPC - Ingeniería de Software\Ciclo 9\TP1\RelaxationTechniques\DigitalizeRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D2FF19-8E72-4ECB-9F22-7CCF9595266F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7110261-A4AE-48E4-834F-0C4A457FF49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{B0A53B9D-7221-45F2-935E-7C0702C6B0BC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B0A53B9D-7221-45F2-935E-7C0702C6B0BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tecnicas" sheetId="1" r:id="rId1"/>
@@ -828,9 +828,6 @@
     <t>https://github.com/GabrielGomezDlc/TechniquesAudios/raw/refs/heads/main/Mindfulness/49-meditacionatencionarespiracion-canalestoesmbtb-ivoox102476807.mp3</t>
   </si>
   <si>
-    <t>https://github.com/GabrielGomezDlc/TechniquesAudios/blob/main/Mindfulness/50-Meditacion%20Guiada%20de%20Paz.mp3</t>
-  </si>
-  <si>
     <t>https://github.com/GabrielGomezDlc/TechniquesAudios/raw/refs/heads/main/Musictherapies/51-meditative-rain.mp3</t>
   </si>
   <si>
@@ -901,6 +898,9 @@
   </si>
   <si>
     <t>https://github.com/GabrielGomezDlc/TechniquesAudios/raw/refs/heads/main/Musictherapies/75-meditation-amp-relax-238980.mp3</t>
+  </si>
+  <si>
+    <t>https://github.com/GabrielGomezDlc/TechniquesAudios/raw/refs/heads/main/Mindfulness/50-Meditacion%20Guiada%20de%20Paz.mp3</t>
   </si>
 </sst>
 </file>
@@ -2173,8 +2173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D22D24-AFBA-4774-8152-CCECE65B93D4}">
   <dimension ref="A1:G156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F153" sqref="F153"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G131" sqref="G131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -4340,8 +4340,8 @@
       <c r="C131" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G131" t="s">
-        <v>263</v>
+      <c r="G131" s="2" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -4355,7 +4355,7 @@
         <v>78</v>
       </c>
       <c r="G132" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -4369,7 +4369,7 @@
         <v>78</v>
       </c>
       <c r="G133" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -4383,7 +4383,7 @@
         <v>78</v>
       </c>
       <c r="G134" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -4397,7 +4397,7 @@
         <v>78</v>
       </c>
       <c r="G135" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -4411,7 +4411,7 @@
         <v>78</v>
       </c>
       <c r="G136" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -4425,7 +4425,7 @@
         <v>78</v>
       </c>
       <c r="G137" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -4439,7 +4439,7 @@
         <v>78</v>
       </c>
       <c r="G138" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -4453,7 +4453,7 @@
         <v>78</v>
       </c>
       <c r="G139" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -4467,7 +4467,7 @@
         <v>78</v>
       </c>
       <c r="G140" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -4481,7 +4481,7 @@
         <v>78</v>
       </c>
       <c r="G141" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -4495,7 +4495,7 @@
         <v>78</v>
       </c>
       <c r="G142" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -4509,7 +4509,7 @@
         <v>78</v>
       </c>
       <c r="G143" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -4523,7 +4523,7 @@
         <v>78</v>
       </c>
       <c r="G144" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="145" spans="1:7">
@@ -4537,7 +4537,7 @@
         <v>78</v>
       </c>
       <c r="G145" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="146" spans="1:7">
@@ -4551,7 +4551,7 @@
         <v>78</v>
       </c>
       <c r="G146" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="147" spans="1:7">
@@ -4565,7 +4565,7 @@
         <v>78</v>
       </c>
       <c r="G147" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="148" spans="1:7">
@@ -4579,7 +4579,7 @@
         <v>78</v>
       </c>
       <c r="G148" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="149" spans="1:7">
@@ -4593,7 +4593,7 @@
         <v>78</v>
       </c>
       <c r="G149" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -4607,7 +4607,7 @@
         <v>78</v>
       </c>
       <c r="G150" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="151" spans="1:7">
@@ -4621,7 +4621,7 @@
         <v>78</v>
       </c>
       <c r="G151" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="152" spans="1:7">
@@ -4635,7 +4635,7 @@
         <v>78</v>
       </c>
       <c r="G152" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -4649,7 +4649,7 @@
         <v>78</v>
       </c>
       <c r="G153" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -4663,7 +4663,7 @@
         <v>78</v>
       </c>
       <c r="G154" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -4677,7 +4677,7 @@
         <v>78</v>
       </c>
       <c r="G155" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -4691,14 +4691,15 @@
         <v>78</v>
       </c>
       <c r="G156" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G107" r:id="rId1" xr:uid="{7C7B2F59-81F4-4F37-9F0F-07DCDC62C6FC}"/>
+    <hyperlink ref="G131" r:id="rId2" xr:uid="{407330B5-89A3-4930-B3DF-46BD96255C9A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>